<commit_message>
- add switch "-b" - add capacity report without buckets details
</commit_message>
<xml_diff>
--- a/ecs_capacities.xlsx
+++ b/ecs_capacities.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F383"/>
+  <dimension ref="A1:I383"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,6 +442,21 @@
           <t>22-Jun-2021 (16:22:37)</t>
         </is>
       </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>22-Jun-2021 (22:33:35)</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>22-Jun-2021 (22:41:03)</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>22-Jun-2021 (22:41:32)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -466,6 +481,15 @@
       <c r="F2" t="n">
         <v>362602613.9648</v>
       </c>
+      <c r="G2" t="n">
+        <v>362602613.9648</v>
+      </c>
+      <c r="H2" t="n">
+        <v>362602613.9648</v>
+      </c>
+      <c r="I2" t="n">
+        <v>362602613.9648</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -490,6 +514,15 @@
       <c r="F3" t="n">
         <v>0</v>
       </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -514,6 +547,15 @@
       <c r="F4" t="n">
         <v>0</v>
       </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -538,6 +580,15 @@
       <c r="F5" t="n">
         <v>0</v>
       </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -562,6 +613,15 @@
       <c r="F6" t="n">
         <v>0</v>
       </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -586,6 +646,15 @@
       <c r="F7" t="n">
         <v>0</v>
       </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -610,6 +679,15 @@
       <c r="F8" t="n">
         <v>0</v>
       </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -634,6 +712,15 @@
       <c r="F9" t="n">
         <v>0</v>
       </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -752,6 +839,15 @@
         <v>0</v>
       </c>
       <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>